<commit_message>
added comments showing that which column is which
</commit_message>
<xml_diff>
--- a/en-ar.xlsx
+++ b/en-ar.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="104">
   <si>
     <t>en</t>
   </si>
@@ -286,6 +286,9 @@
     <t>He has a bank commitment</t>
   </si>
   <si>
+    <t>Test Translation Bundle Automation</t>
+  </si>
+  <si>
     <t>Test Form</t>
   </si>
   <si>
@@ -305,6 +308,9 @@
   </si>
   <si>
     <t>Submit</t>
+  </si>
+  <si>
+    <t>اختبار أتمتة حزمة الترجمة</t>
   </si>
   <si>
     <t>نموذج الاختبار</t>
@@ -332,7 +338,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,17 +360,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Sakkal Majalla"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF9C590B"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -493,19 +488,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
@@ -525,9 +514,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,349 +800,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B75"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.77734375" customWidth="1"/>
-    <col min="2" max="2" width="75.5546875" customWidth="1"/>
-    <col min="3" max="3" width="67" customWidth="1"/>
+    <col min="1" max="1" width="66.77734375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="75.5546875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="67" style="10" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="5"/>
-    </row>
-    <row r="19" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="5"/>
-    </row>
-    <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="5"/>
-    </row>
-    <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:2" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="5"/>
-    </row>
-    <row r="24" spans="1:2" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:2" ht="101.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:2" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="8"/>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9"/>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9"/>
-      <c r="B30" s="3"/>
-    </row>
-    <row r="31" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="3"/>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9"/>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9"/>
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="10"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9"/>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9"/>
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9"/>
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9"/>
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9"/>
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9"/>
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9"/>
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="9"/>
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="9"/>
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="1:2" ht="19.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47" s="11"/>
-    </row>
-    <row r="48" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="4"/>
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4"/>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="4"/>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="4"/>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4"/>
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="4"/>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="4"/>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="4"/>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="4"/>
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="4"/>
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="4"/>
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="4"/>
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="4"/>
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="4"/>
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="4"/>
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="4"/>
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A72" s="4"/>
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="4"/>
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="4"/>
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="4"/>
-      <c r="B75" s="3"/>
-    </row>
+      <c r="B9" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" ht="43.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="43.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="58.2" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="101.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="43.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -1173,354 +912,354 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="2" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="2" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>